<commit_message>
container, individual, comments extraction
</commit_message>
<xml_diff>
--- a/data/MOH-TEST.xlsx
+++ b/data/MOH-TEST.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="126">
   <si>
     <t xml:space="preserve">McGill Genome Center Sample Manifest version [1.1.1] - 2021-09-20</t>
   </si>
@@ -738,6 +738,9 @@
   </si>
   <si>
     <t xml:space="preserve">MoHQ-CM-1-1-1041-1-D-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris</t>
   </si>
   <si>
     <t xml:space="preserve">96 well plate</t>
@@ -1685,9 +1688,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>923400</xdr:colOff>
+      <xdr:colOff>923040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1701,7 +1704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="837000" y="216000"/>
-          <a:ext cx="3614400" cy="850680"/>
+          <a:ext cx="3614040" cy="850320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6371,11 +6374,11 @@
   </sheetPr>
   <dimension ref="A1:AG392"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T11" activeCellId="0" sqref="T11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
@@ -6978,35 +6981,37 @@
         <v>62</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="22" t="s">
+        <v>63</v>
+      </c>
       <c r="F9" s="23" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
       <c r="N9" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O9" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N9,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P9" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
@@ -7019,7 +7024,7 @@
         <v>50.299</v>
       </c>
       <c r="X9" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
@@ -7039,42 +7044,44 @@
         <v>61</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="E10" s="27" t="s">
+        <v>63</v>
+      </c>
       <c r="F10" s="23" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
       <c r="N10" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O10" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N10,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P10" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R10" s="23"/>
       <c r="S10" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
@@ -7085,7 +7092,7 @@
         <v>39.06</v>
       </c>
       <c r="X10" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y10" s="23"/>
       <c r="Z10" s="23"/>
@@ -7105,42 +7112,44 @@
         <v>61</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
+      <c r="E11" s="27" t="s">
+        <v>63</v>
+      </c>
       <c r="F11" s="23" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O11" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N11,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R11" s="23"/>
       <c r="S11" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
@@ -7151,7 +7160,7 @@
         <v>61.447</v>
       </c>
       <c r="X11" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y11" s="23"/>
       <c r="Z11" s="23"/>
@@ -7171,7 +7180,7 @@
         <v>61</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="27"/>
@@ -7179,34 +7188,34 @@
         <v>1</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
       <c r="N12" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O12" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N12,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P12" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R12" s="23"/>
       <c r="S12" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
@@ -7217,7 +7226,7 @@
         <v>84.933</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y12" s="23"/>
       <c r="Z12" s="23"/>
@@ -7237,7 +7246,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="27"/>
@@ -7245,34 +7254,34 @@
         <v>1</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O13" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N13,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R13" s="23"/>
       <c r="S13" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T13" s="19"/>
       <c r="U13" s="19"/>
@@ -7283,7 +7292,7 @@
         <v>63.727</v>
       </c>
       <c r="X13" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y13" s="23"/>
       <c r="Z13" s="23"/>
@@ -7303,7 +7312,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
@@ -7311,34 +7320,34 @@
         <v>1</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O14" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N14,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P14" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R14" s="23"/>
       <c r="S14" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
@@ -7349,7 +7358,7 @@
         <v>28.397</v>
       </c>
       <c r="X14" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y14" s="23"/>
       <c r="Z14" s="23"/>
@@ -7369,7 +7378,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="27"/>
@@ -7377,34 +7386,34 @@
         <v>1</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
       <c r="N15" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O15" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N15,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P15" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R15" s="23"/>
       <c r="S15" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
@@ -7415,7 +7424,7 @@
         <v>15.399</v>
       </c>
       <c r="X15" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y15" s="23"/>
       <c r="Z15" s="23"/>
@@ -7435,7 +7444,7 @@
         <v>61</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="27"/>
@@ -7443,34 +7452,34 @@
         <v>1</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O16" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N16,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P16" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R16" s="23"/>
       <c r="S16" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T16" s="19"/>
       <c r="U16" s="19"/>
@@ -7481,7 +7490,7 @@
         <v>164.701</v>
       </c>
       <c r="X16" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y16" s="23"/>
       <c r="Z16" s="23"/>
@@ -7492,7 +7501,7 @@
       <c r="AE16" s="28"/>
       <c r="AF16" s="28"/>
       <c r="AG16" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7503,7 +7512,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="27"/>
@@ -7511,34 +7520,34 @@
         <v>1</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
       <c r="N17" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O17" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N17,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R17" s="23"/>
       <c r="S17" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T17" s="19"/>
       <c r="U17" s="19"/>
@@ -7549,7 +7558,7 @@
         <v>195.386</v>
       </c>
       <c r="X17" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y17" s="23"/>
       <c r="Z17" s="23"/>
@@ -7560,7 +7569,7 @@
       <c r="AE17" s="28"/>
       <c r="AF17" s="28"/>
       <c r="AG17" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7571,7 +7580,7 @@
         <v>61</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="27"/>
@@ -7579,34 +7588,34 @@
         <v>1</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
       <c r="N18" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O18" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N18,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P18" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R18" s="23"/>
       <c r="S18" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T18" s="19"/>
       <c r="U18" s="19"/>
@@ -7617,7 +7626,7 @@
         <v>147.407</v>
       </c>
       <c r="X18" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y18" s="23"/>
       <c r="Z18" s="23"/>
@@ -7628,7 +7637,7 @@
       <c r="AE18" s="28"/>
       <c r="AF18" s="28"/>
       <c r="AG18" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7639,7 +7648,7 @@
         <v>61</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="27"/>
@@ -7647,34 +7656,34 @@
         <v>1</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O19" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N19,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P19" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R19" s="23"/>
       <c r="S19" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
@@ -7685,7 +7694,7 @@
         <v>117.948</v>
       </c>
       <c r="X19" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y19" s="23"/>
       <c r="Z19" s="23"/>
@@ -7696,7 +7705,7 @@
       <c r="AE19" s="28"/>
       <c r="AF19" s="28"/>
       <c r="AG19" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7707,7 +7716,7 @@
         <v>61</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
@@ -7715,34 +7724,34 @@
         <v>1</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O20" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N20,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P20" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R20" s="23"/>
       <c r="S20" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T20" s="19"/>
       <c r="U20" s="19"/>
@@ -7753,7 +7762,7 @@
         <v>141.72</v>
       </c>
       <c r="X20" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y20" s="23"/>
       <c r="Z20" s="23"/>
@@ -7764,7 +7773,7 @@
       <c r="AE20" s="28"/>
       <c r="AF20" s="28"/>
       <c r="AG20" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7775,7 +7784,7 @@
         <v>61</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
@@ -7783,34 +7792,34 @@
         <v>1</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O21" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N21,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P21" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q21" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R21" s="23"/>
       <c r="S21" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T21" s="19"/>
       <c r="U21" s="19"/>
@@ -7821,7 +7830,7 @@
         <v>157.89</v>
       </c>
       <c r="X21" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y21" s="23"/>
       <c r="Z21" s="23"/>
@@ -7832,7 +7841,7 @@
       <c r="AE21" s="28"/>
       <c r="AF21" s="28"/>
       <c r="AG21" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7843,7 +7852,7 @@
         <v>61</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
@@ -7851,34 +7860,34 @@
         <v>1</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O22" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N22,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P22" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q22" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R22" s="23"/>
       <c r="S22" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T22" s="19"/>
       <c r="U22" s="19"/>
@@ -7889,7 +7898,7 @@
         <v>133.734</v>
       </c>
       <c r="X22" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y22" s="23"/>
       <c r="Z22" s="23"/>
@@ -7900,7 +7909,7 @@
       <c r="AE22" s="28"/>
       <c r="AF22" s="28"/>
       <c r="AG22" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" s="10" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7911,7 +7920,7 @@
         <v>61</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
@@ -7919,42 +7928,42 @@
         <v>1</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J23" s="19"/>
       <c r="K23" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M23" s="19"/>
       <c r="N23" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O23" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N23,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P23" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R23" s="23"/>
       <c r="S23" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T23" s="19"/>
       <c r="U23" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V23" s="19" t="n">
         <v>15</v>
@@ -7963,7 +7972,7 @@
         <v>113.981</v>
       </c>
       <c r="X23" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y23" s="23"/>
       <c r="Z23" s="23"/>
@@ -7983,7 +7992,7 @@
         <v>61</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
@@ -7991,42 +8000,42 @@
         <v>1</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J24" s="19"/>
       <c r="K24" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O24" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N24,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P24" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R24" s="23"/>
       <c r="S24" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T24" s="19"/>
       <c r="U24" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V24" s="19" t="n">
         <v>15</v>
@@ -8035,7 +8044,7 @@
         <v>61.351</v>
       </c>
       <c r="X24" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y24" s="23"/>
       <c r="Z24" s="23"/>
@@ -8055,7 +8064,7 @@
         <v>61</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
@@ -8063,42 +8072,42 @@
         <v>1</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J25" s="19"/>
       <c r="K25" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O25" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N25,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P25" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q25" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R25" s="23"/>
       <c r="S25" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T25" s="19"/>
       <c r="U25" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V25" s="19" t="n">
         <v>15</v>
@@ -8107,7 +8116,7 @@
         <v>237.872</v>
       </c>
       <c r="X25" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y25" s="23"/>
       <c r="Z25" s="23"/>
@@ -8127,7 +8136,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
@@ -8135,42 +8144,42 @@
         <v>1</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M26" s="19"/>
       <c r="N26" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O26" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N26,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P26" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R26" s="23"/>
       <c r="S26" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T26" s="19"/>
       <c r="U26" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V26" s="19" t="n">
         <v>15</v>
@@ -8179,7 +8188,7 @@
         <v>297.898</v>
       </c>
       <c r="X26" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y26" s="23"/>
       <c r="Z26" s="23"/>
@@ -8199,7 +8208,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="27"/>
@@ -8207,42 +8216,42 @@
         <v>1</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J27" s="19"/>
       <c r="K27" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M27" s="19"/>
       <c r="N27" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O27" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N27,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P27" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R27" s="23"/>
       <c r="S27" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T27" s="19"/>
       <c r="U27" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V27" s="19" t="n">
         <v>15</v>
@@ -8251,7 +8260,7 @@
         <v>287.512</v>
       </c>
       <c r="X27" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y27" s="23"/>
       <c r="Z27" s="23"/>
@@ -8271,7 +8280,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
@@ -8279,42 +8288,42 @@
         <v>1</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J28" s="19"/>
       <c r="K28" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M28" s="19"/>
       <c r="N28" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O28" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N28,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P28" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q28" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R28" s="23"/>
       <c r="S28" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T28" s="19"/>
       <c r="U28" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V28" s="19" t="n">
         <v>15</v>
@@ -8323,7 +8332,7 @@
         <v>127.289</v>
       </c>
       <c r="X28" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y28" s="23"/>
       <c r="Z28" s="23"/>
@@ -8343,7 +8352,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="27"/>
@@ -8351,42 +8360,42 @@
         <v>1</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M29" s="19"/>
       <c r="N29" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O29" s="25" t="n">
         <f aca="false">IFERROR(VLOOKUP(N29,[1]ranges!N$2:P$422,3,0),"")</f>
         <v>3257.32</v>
       </c>
       <c r="P29" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R29" s="23"/>
       <c r="S29" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T29" s="19"/>
       <c r="U29" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V29" s="19" t="n">
         <v>15</v>
@@ -8395,7 +8404,7 @@
         <v>51.836</v>
       </c>
       <c r="X29" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y29" s="23"/>
       <c r="Z29" s="23"/>

</xml_diff>